<commit_message>
It passes all test with data from excel file
</commit_message>
<xml_diff>
--- a/ReadingData/sample.xlsx
+++ b/ReadingData/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\Version2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\ReadingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE3D2B-A964-43BE-816D-81A6A915DFAD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC81C8B6-674F-4A1D-9FE2-879BB654B391}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10211" xr2:uid="{F790CF26-CA6A-49AA-84C8-390D6428DC29}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
   <si>
     <t>color</t>
   </si>
@@ -120,24 +120,9 @@
     <t>worms</t>
   </si>
   <si>
-    <t>Apple_feature</t>
-  </si>
-  <si>
-    <t>Apple_val</t>
-  </si>
-  <si>
     <t>Concepts</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>Bowl</t>
-  </si>
-  <si>
-    <t>Bowl_feature</t>
-  </si>
-  <si>
     <t>eat</t>
   </si>
   <si>
@@ -207,9 +192,6 @@
     <t>cup</t>
   </si>
   <si>
-    <t>Bowl_val</t>
-  </si>
-  <si>
     <t>cup_feature</t>
   </si>
   <si>
@@ -352,6 +334,27 @@
   </si>
   <si>
     <t>round_end</t>
+  </si>
+  <si>
+    <t>bowl_feature</t>
+  </si>
+  <si>
+    <t>bowl_val</t>
+  </si>
+  <si>
+    <t>apple_feature</t>
+  </si>
+  <si>
+    <t>apple_val</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>bowl</t>
+  </si>
+  <si>
+    <t>spoon</t>
   </si>
 </sst>
 </file>
@@ -713,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF85D927-26DA-4A2C-99F1-700451991764}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12:S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05"/>
@@ -729,66 +732,66 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
         <v>87</v>
       </c>
-      <c r="N2" t="s">
-        <v>93</v>
-      </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="Q2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="R2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -806,19 +809,19 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
         <v>16</v>
@@ -830,24 +833,24 @@
         <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="P3" t="s">
         <v>2</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="R3" t="s">
         <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -859,54 +862,54 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N4" t="s">
         <v>11</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="P4" t="s">
         <v>11</v>
       </c>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="R4" t="s">
         <v>2</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -918,54 +921,54 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
       <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
         <v>38</v>
       </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>43</v>
-      </c>
       <c r="R5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="S5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -977,54 +980,54 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N6" t="s">
         <v>11</v>
       </c>
       <c r="O6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P6" t="s">
         <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="R6" t="s">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -1036,54 +1039,54 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P7" t="s">
         <v>16</v>
       </c>
       <c r="Q7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="R7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="S7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1095,31 +1098,31 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="N8" t="s">
         <v>16</v>
@@ -1128,21 +1131,21 @@
         <v>17</v>
       </c>
       <c r="P8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="Q8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="R8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="S8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -1151,57 +1154,57 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
       </c>
       <c r="Q9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="R9" t="s">
         <v>25</v>
       </c>
       <c r="S9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -1210,55 +1213,58 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N10" t="s">
         <v>2</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="P10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="Q10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="R10" t="s">
         <v>11</v>
       </c>
       <c r="S10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:19">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1269,37 +1275,37 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L11" t="s">
         <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="P11" t="s">
         <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="R11" t="s">
         <v>11</v>
       </c>
       <c r="S11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1313,37 +1319,37 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="P12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="Q12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="R12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="S12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1357,19 +1363,19 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J13" t="s">
         <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="P13" t="s">
         <v>25</v>
       </c>
       <c r="Q13" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1383,19 +1389,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="P14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="Q14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1406,10 +1412,10 @@
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:19">

</xml_diff>

<commit_message>
Modify a bit some programs and finish with FEATS_brm.xls file
</commit_message>
<xml_diff>
--- a/ReadingData/sample.xlsx
+++ b/ReadingData/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\ReadingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC81C8B6-674F-4A1D-9FE2-879BB654B391}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEFD21C-39E4-4321-ADA1-57CE29D3DFBD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10211" xr2:uid="{F790CF26-CA6A-49AA-84C8-390D6428DC29}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="123">
   <si>
     <t>color</t>
   </si>
@@ -225,9 +225,6 @@
     <t>sharp</t>
   </si>
   <si>
-    <t>stainless_steel</t>
-  </si>
-  <si>
     <t>knife</t>
   </si>
   <si>
@@ -355,6 +352,48 @@
   </si>
   <si>
     <t>spoon</t>
+  </si>
+  <si>
+    <t>handle_feature</t>
+  </si>
+  <si>
+    <t>handle_val</t>
+  </si>
+  <si>
+    <t>metal_feature</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>ceramic_feature</t>
+  </si>
+  <si>
+    <t>plastic_feature</t>
+  </si>
+  <si>
+    <t>glass_feature</t>
+  </si>
+  <si>
+    <t>transparent</t>
+  </si>
+  <si>
+    <t>steel_feature</t>
+  </si>
+  <si>
+    <t>metal_val</t>
+  </si>
+  <si>
+    <t>ceramic_val</t>
+  </si>
+  <si>
+    <t>plastic_val</t>
+  </si>
+  <si>
+    <t>glass_val</t>
+  </si>
+  <si>
+    <t>steel_val</t>
   </si>
 </sst>
 </file>
@@ -714,37 +753,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF85D927-26DA-4A2C-99F1-700451991764}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05"/>
   <cols>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="24" max="24" width="14.21875" customWidth="1"/>
+    <col min="25" max="25" width="12.77734375" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:31">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
-        <v>106</v>
-      </c>
       <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
         <v>103</v>
-      </c>
-      <c r="E2" t="s">
-        <v>104</v>
       </c>
       <c r="F2" t="s">
         <v>55</v>
@@ -759,39 +805,75 @@
         <v>59</v>
       </c>
       <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
         <v>68</v>
       </c>
-      <c r="K2" t="s">
-        <v>69</v>
-      </c>
       <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
         <v>80</v>
       </c>
-      <c r="M2" t="s">
-        <v>81</v>
-      </c>
       <c r="N2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" t="s">
         <v>87</v>
       </c>
-      <c r="O2" t="s">
-        <v>88</v>
-      </c>
       <c r="P2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>99</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>100</v>
       </c>
-      <c r="S2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" t="s">
+        <v>111</v>
+      </c>
+      <c r="W2" t="s">
+        <v>118</v>
+      </c>
+      <c r="X2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -833,7 +915,7 @@
         <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P3" t="s">
         <v>2</v>
@@ -847,10 +929,46 @@
       <c r="S3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T3" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -880,7 +998,7 @@
         <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L4" t="s">
         <v>37</v>
@@ -906,8 +1024,44 @@
       <c r="S4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>112</v>
+      </c>
+      <c r="X4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -965,8 +1119,38 @@
       <c r="S5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>44</v>
+      </c>
+      <c r="X5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -998,7 +1182,7 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s">
         <v>37</v>
@@ -1010,24 +1194,30 @@
         <v>11</v>
       </c>
       <c r="O6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P6" t="s">
         <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R6" t="s">
         <v>0</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>112</v>
+      </c>
+      <c r="T6" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -1057,13 +1247,13 @@
         <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N7" t="s">
         <v>39</v>
@@ -1075,18 +1265,18 @@
         <v>16</v>
       </c>
       <c r="Q7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R7" t="s">
         <v>37</v>
       </c>
       <c r="S7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1113,7 +1303,7 @@
         <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
         <v>61</v>
@@ -1122,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N8" t="s">
         <v>16</v>
@@ -1143,9 +1333,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -1181,10 +1371,10 @@
         <v>39</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O9" t="s">
         <v>51</v>
@@ -1193,7 +1383,7 @@
         <v>25</v>
       </c>
       <c r="Q9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R9" t="s">
         <v>25</v>
@@ -1202,9 +1392,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -1228,13 +1418,13 @@
         <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
         <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L10" t="s">
         <v>37</v>
@@ -1258,12 +1448,12 @@
         <v>11</v>
       </c>
       <c r="S10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
@@ -1287,19 +1477,19 @@
         <v>37</v>
       </c>
       <c r="K11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
         <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P11" t="s">
         <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R11" t="s">
         <v>11</v>
@@ -1308,7 +1498,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:31">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1343,7 +1536,7 @@
         <v>37</v>
       </c>
       <c r="Q12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R12" t="s">
         <v>37</v>
@@ -1352,7 +1545,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:31">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1369,16 +1565,19 @@
         <v>2</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
         <v>25</v>
       </c>
       <c r="Q13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1392,19 +1591,22 @@
         <v>44</v>
       </c>
       <c r="J14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" t="s">
         <v>77</v>
       </c>
-      <c r="K14" t="s">
-        <v>78</v>
-      </c>
       <c r="P14" t="s">
         <v>37</v>
       </c>
       <c r="Q14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1620,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:31">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1426,7 +1631,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1434,7 +1642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="1:3">
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1442,7 +1650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="1:3">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="1:3">
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1458,7 +1666,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="1:3">
       <c r="B21" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>